<commit_message>
updated with log config
</commit_message>
<xml_diff>
--- a/Master Sheet.xlsx
+++ b/Master Sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>https://play.google.com/store/apps/details?id=com.astroshaadi.customer</t>
   </si>
@@ -259,6 +259,99 @@
   </si>
   <si>
     <t>https://play.google.com/store/apps/details?id=ai.photoeditor.artgenerator</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.ucmqed.peqqus</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.upticker.app.v2</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.digitaljungle</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.advanced.voiceChanger</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.app.malgopay</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.machi.call.ChatLiveCall.mochi</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=co.sansa.vhgmw</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.astropower.user</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.fotoapp.perfectme.bodyshape.photoeditor.bodyeditor</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.mb.hexasort.coinstackgame</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=antitheftalarm.donttouchmyphone.antipro</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=dailybend.bend.stretch.flexibility.fitness.exercise.back</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=photo.video.maker.editor</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=pl.idreams.SkyForceReloaded</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.fakecall.prankcall.videocall.voicechat</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.aamdhane.app</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.idramas.tv</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.trackmyphone.find.myphone.phonelocator.antitheft</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.earthvibe.wall</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.eventbeep.android</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.wowchat.wallet</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.smartearn.gpstracker</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=xyz.multipl.multipl</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.live.map.earth.app</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.appspelago.peekababy</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.qr.cvn.barcode.scanner.fhnn</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.happyverse.spellinggame</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.prank.crazy.trickly.aos</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=grocery.beldara.fresh</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.tnibro</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.navigation.offlinemaps.radar.fortravel</t>
   </si>
 </sst>
 </file>
@@ -577,7 +670,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A80"/>
+  <dimension ref="A1:A111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
@@ -985,6 +1078,161 @@
         <v>79</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="0">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="0">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="0">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="0">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="0">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="0">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="0">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="0">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="0">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="0">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="0">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="0">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="0">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="0">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="0">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="0">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="0">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="0">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>